<commit_message>
Partial overview computation times
</commit_message>
<xml_diff>
--- a/06.Paper Material/Computation times.xlsx
+++ b/06.Paper Material/Computation times.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>3bus</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>Comp time</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>nb cores</t>
+  </si>
+  <si>
+    <t>cpu time/mode</t>
   </si>
 </sst>
 </file>
@@ -369,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,73 +396,210 @@
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4">
+        <v>39075</v>
+      </c>
+      <c r="D4">
+        <v>6346</v>
+      </c>
+      <c r="G4">
+        <v>677960</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>2843875</v>
+      </c>
+      <c r="J4">
+        <v>36</v>
+      </c>
+      <c r="L4">
+        <v>36</v>
+      </c>
+      <c r="M4">
+        <v>72</v>
+      </c>
+      <c r="P4">
+        <f>C4/L4</f>
+        <v>1085.4166666666667</v>
+      </c>
+      <c r="Q4">
+        <f>D4/M4</f>
+        <v>88.138888888888886</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C7">
+        <v>1336</v>
+      </c>
+      <c r="D7">
+        <v>20301</v>
+      </c>
+      <c r="G7">
+        <v>121496</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1620835</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="P7">
+        <f>C7/L7</f>
+        <v>111.33333333333333</v>
+      </c>
+      <c r="Q7">
+        <f>D7/M7</f>
+        <v>1691.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="D10">
+        <v>4427</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>405217</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>36</v>
+      </c>
+      <c r="P10" t="e">
+        <f>C10/L10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q10">
+        <f>D10/M10</f>
+        <v>122.97222222222223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>